<commit_message>
Added new PRM functions for MovesetPlus addon
</commit_message>
<xml_diff>
--- a/bin/Debug/moddingAPI_files/moddingapi/mods/movesetplus/Function Documentation.xlsx
+++ b/bin/Debug/moddingAPI_files/moddingapi/mods/movesetplus/Function Documentation.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\NARUTO SHIPPUDEN Ultimate Ninja STORM 4\moddingapi\mods\movesetplus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Steam(2)\steamapps\common\NARUTO SHIPPUDEN Ultimate Ninja STORM 4\moddingapi\mods\movesetplus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F648400-A17D-4C32-BE7B-CF9AB941C455}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D4F3CE7E-55C7-47D7-ACCD-2CC9C63C145F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>FUNCTION NAME</t>
   </si>
@@ -455,17 +454,128 @@
 EC 00 07 00 02 00 00 00 00 00 00 00 C8 42 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00</t>
     </r>
   </si>
+  <si>
+    <t>EC09 - MOT_UPGRADE</t>
+  </si>
+  <si>
+    <t>Set the function to EC, and the first parameter to 9.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The second parameter decides what moveset will be used.
+0 = Normal state moveset
+1 = Awakening state moveset
+2 = upgrade01 moveset
+3 = upgrade02 moveset
+4 = upgrade03 moveset
+5 = boss01 moveset
+6 = boss02 moveset
+7 = boss03 moveset
+8 = boss04 moveset
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Example: You want to use upgrade03 moveset.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Function is EC, PARAM1 is 9, PARAM3 is 4.
+EC 00 09 00 04 00 00 00 00 00 00 00 00 00</t>
+    </r>
+  </si>
+  <si>
+    <t>EC0A - DISABLE_ENABLE_BGM</t>
+  </si>
+  <si>
+    <t>This function let you stop or start playing BGM which was played on stage.</t>
+  </si>
+  <si>
+    <t>Set the function to EC, and the first parameter to A.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The second parameter decides disable or enable BGM.
+0 = Disable
+1 = Enable
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example: You want to enable BGM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Function is EC, PARAM1 is A, PARAM2 is 1
+EC 00 0A 00 01 00 00 00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Same as MOT_UPGRADE, but was improved. Now when you using that function, moveset will be unchanged after attack (like with Kaguya). Were added new slots for switching. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(CURRENTLY DISABLED)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -512,8 +622,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,8 +655,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -560,29 +685,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="2" builtinId="10"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Примечание" xfId="2" builtinId="10"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -893,14 +1036,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76333E04-CAED-49D8-AC14-1BBFB801BE33}">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="48.28515625" customWidth="1"/>
@@ -909,146 +1052,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="195" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="195" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="195" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>